<commit_message>
[Silverfox] Company 목록 갱신
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/회사.xlsx
+++ b/DesignDocs/Design/회사.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32956D14-51F0-468E-9246-8A1988137255}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6978D4FB-6320-4CE2-8C8F-391F72409C02}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11190" xr2:uid="{0E1B0CCF-CA20-4CE0-9D34-302DB824E1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,15 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Walker's Workshop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Smith's Smithy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>cid</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -55,49 +50,22 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Delicate Bastard</t>
-  </si>
-  <si>
     <t>섬세한 불한당</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>검은 증기 공업</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black Steam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pro-Industrial</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>프로 공업소</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Kana-Kooler</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>카나 쿨러</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Raccoon Glass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>라쿤 유리 공예</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>D.S.D.C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>슬럼가 개발 주식회사</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -131,6 +99,58 @@
   </si>
   <si>
     <t>피격시 10% 확률로 데미지 반사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>weak</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>master</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>왕국 연구소</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WalkersWorkshop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SmithsSmithy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DelicateBastard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RoyalLab</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProIndustrial</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KanaKooler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RaccoonGlass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSDC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -506,115 +526,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC990441-06B3-418F-95E6-1E473E5EF571}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.125" customWidth="1"/>
     <col min="3" max="3" width="21.125" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>